<commit_message>
Update policy comparison results
</commit_message>
<xml_diff>
--- a/data/policy_comparison_data.xlsx
+++ b/data/policy_comparison_data.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,6 +522,81 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>573</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://al-policies.exploremyplan.com/portal/web/medical-policies/-/mp-573</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://stage-us-mypolicies.itilitihealth.us/policy/938125692074/573?lob=BCBS+AL</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>573</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://al-policies.exploremyplan.com/portal/web/medical-policies/-/mp-573</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://stage-us-mypolicies.itilitihealth.us/policy/938125692074/573?lob=BCBS+AL</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>573</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://al-policies.exploremyplan.com/portal/web/medical-policies/-/mp-573</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://stage-us-mypolicies.itilitihealth.us/policy/938125692074/573?lob=BCBS+AL</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>573</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://al-policies.exploremyplan.com/portal/web/medical-policies/-/mp-573</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://stage-us-mypolicies.itilitihealth.us/policy/938125692074/573?lob=BCBS+AL</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>573</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://al-policies.exploremyplan.com/portal/web/medical-policies/-/mp-573</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://stage-us-mypolicies.itilitihealth.us/policy/938125692074/573?lob=BCBS+AL</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>